<commit_message>
Keep copy of my different test sketches
</commit_message>
<xml_diff>
--- a/arduino_uno_r4.xlsx
+++ b/arduino_uno_r4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\UNOR4-stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BE1FC6D-E38B-434A-9CF7-DEEFFEFB9E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BBCFA4-2BAB-4531-9663-747D7B1FE69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9930" yWindow="0" windowWidth="26115" windowHeight="20985" activeTab="2" xr2:uid="{8DF1AF20-4F17-4E13-BB05-CAA1D9B0E58D}"/>
+    <workbookView xWindow="11085" yWindow="0" windowWidth="24960" windowHeight="20985" activeTab="1" xr2:uid="{8DF1AF20-4F17-4E13-BB05-CAA1D9B0E58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Table033 (Page 23-26)" sheetId="2" r:id="rId1"/>
@@ -1210,7 +1210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1227,6 +1227,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1252,7 +1258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1260,11 +1266,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="67">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1346,10 +1374,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1543,10 +1567,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{3CA5437F-C535-4DC8-91A8-22D434362B0F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="28" unboundColumnsLeft="2">
@@ -1704,53 +1724,53 @@
     <tableColumn id="10" xr3:uid="{7CC39A3B-515E-4F8C-A6F7-2280B6C92DA1}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="39"/>
     <tableColumn id="3" xr3:uid="{A203754E-A450-4494-B6A5-44EF19BB1F8E}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="38"/>
     <tableColumn id="8" xr3:uid="{4E09F24F-5659-4905-A86D-23D48584A50A}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{EB3BAAA4-603C-40A6-9A4D-EC07A314AB5F}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{EB8A4512-2FDE-4FB0-B0DD-B6191ED09EEC}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="35"/>
-    <tableColumn id="12" xr3:uid="{CF016CEA-ADC5-44A8-B471-E63CA06286F3}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="34"/>
-    <tableColumn id="13" xr3:uid="{03E303EA-BF53-4F11-9DFA-1521FD43EB15}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="33"/>
-    <tableColumn id="14" xr3:uid="{C270C11F-4E2D-4E82-B1CC-0D68C3F1E880}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="32"/>
-    <tableColumn id="15" xr3:uid="{924B7926-CE59-4F31-AEED-2A32DF639D07}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="31"/>
-    <tableColumn id="16" xr3:uid="{F8FF5AAA-2E01-4762-A7A4-7E6F70376AAC}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="30"/>
-    <tableColumn id="17" xr3:uid="{D8E79A77-64C2-48C9-BB71-6D9C19FC3A1C}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="29"/>
-    <tableColumn id="18" xr3:uid="{C21D94B2-836A-4261-84CC-175D3F1E3353}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="28"/>
-    <tableColumn id="19" xr3:uid="{AC93E674-375E-4052-9969-9375BF1FD3A4}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="27"/>
-    <tableColumn id="20" xr3:uid="{B49C16CD-61A2-4F25-B45A-AFA4AAF0FC58}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="26"/>
-    <tableColumn id="21" xr3:uid="{D903978F-23DB-4B03-B7C9-BA809A44B21A}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="25"/>
-    <tableColumn id="22" xr3:uid="{81FBFEBF-D122-4513-86BC-F3847A1B490E}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="24"/>
-    <tableColumn id="23" xr3:uid="{14414913-AA39-4879-8F72-350C915855C1}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="23"/>
-    <tableColumn id="24" xr3:uid="{8CFBBC26-4A1C-44FE-BEDF-C020182C87C6}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{EB3BAAA4-603C-40A6-9A4D-EC07A314AB5F}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{EB8A4512-2FDE-4FB0-B0DD-B6191ED09EEC}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="36"/>
+    <tableColumn id="12" xr3:uid="{CF016CEA-ADC5-44A8-B471-E63CA06286F3}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="35"/>
+    <tableColumn id="13" xr3:uid="{03E303EA-BF53-4F11-9DFA-1521FD43EB15}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="34"/>
+    <tableColumn id="14" xr3:uid="{C270C11F-4E2D-4E82-B1CC-0D68C3F1E880}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="33"/>
+    <tableColumn id="15" xr3:uid="{924B7926-CE59-4F31-AEED-2A32DF639D07}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="32"/>
+    <tableColumn id="16" xr3:uid="{F8FF5AAA-2E01-4762-A7A4-7E6F70376AAC}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="31"/>
+    <tableColumn id="17" xr3:uid="{D8E79A77-64C2-48C9-BB71-6D9C19FC3A1C}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="30"/>
+    <tableColumn id="18" xr3:uid="{C21D94B2-836A-4261-84CC-175D3F1E3353}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="29"/>
+    <tableColumn id="19" xr3:uid="{AC93E674-375E-4052-9969-9375BF1FD3A4}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="28"/>
+    <tableColumn id="20" xr3:uid="{B49C16CD-61A2-4F25-B45A-AFA4AAF0FC58}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="27"/>
+    <tableColumn id="21" xr3:uid="{D903978F-23DB-4B03-B7C9-BA809A44B21A}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="26"/>
+    <tableColumn id="22" xr3:uid="{81FBFEBF-D122-4513-86BC-F3847A1B490E}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="25"/>
+    <tableColumn id="23" xr3:uid="{14414913-AA39-4879-8F72-350C915855C1}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="24"/>
+    <tableColumn id="24" xr3:uid="{8CFBBC26-4A1C-44FE-BEDF-C020182C87C6}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}" name="Table_Table033__Page_23_263" displayName="Table_Table033__Page_23_263" ref="A1:T22" tableType="queryTable" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}" name="Table_Table033__Page_23_263" displayName="Table_Table033__Page_23_263" ref="A1:T22" tableType="queryTable" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="A1:T22" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="25" xr3:uid="{BE68D2CB-5447-4D49-B30A-0B4C0474174A}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="19"/>
-    <tableColumn id="26" xr3:uid="{84851A1F-0852-4293-AF8E-7CF07D757ECD}" uniqueName="26" name="WIFI" queryTableFieldId="25" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{2E3DDC90-3A23-41DD-AB0D-1BF738911004}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{82C193A7-9F71-4110-B199-955A18BF73C7}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="16"/>
-    <tableColumn id="8" xr3:uid="{8C3AA304-F004-4A71-B050-8AA86784BA22}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{DAAC2DA6-CC15-480F-8376-08C7D49CCFAC}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{ACAFE223-634A-4220-89F7-A4378B0A4CB7}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{D4CFBB7D-1839-4E51-B405-B965D4BD5663}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{56759132-2838-427F-8CEB-7B84D96E48AD}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{763BB52C-9D74-4E50-8283-63C7653A623D}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{056D4100-CE19-456F-886C-346613E23F54}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{86C71EC7-589A-48F4-A94B-B0D31FE60863}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{B2834F24-112D-459F-B770-872CB2D2EA31}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{9ACC56B2-2F1F-47BE-AB93-DAFFAA80F3E3}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="6"/>
-    <tableColumn id="19" xr3:uid="{BA39261E-2C8C-4139-B7E9-00D55BBF4287}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{AFEB0E62-F3EB-4854-B1CA-4A989BA06A87}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{22AF861C-2756-43B7-A352-3E30B03142CE}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{2044D69C-DD13-41EF-8B9B-60D8AEC112FB}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{C74D06FB-AD56-4A98-983F-16DC10955D3B}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{24D5DD84-F585-4F0A-AD0F-1604A8FD60A9}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="0"/>
+    <tableColumn id="25" xr3:uid="{BE68D2CB-5447-4D49-B30A-0B4C0474174A}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="20"/>
+    <tableColumn id="26" xr3:uid="{84851A1F-0852-4293-AF8E-7CF07D757ECD}" uniqueName="26" name="WIFI" queryTableFieldId="25" dataDxfId="19"/>
+    <tableColumn id="10" xr3:uid="{2E3DDC90-3A23-41DD-AB0D-1BF738911004}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{82C193A7-9F71-4110-B199-955A18BF73C7}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{8C3AA304-F004-4A71-B050-8AA86784BA22}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{DAAC2DA6-CC15-480F-8376-08C7D49CCFAC}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="15"/>
+    <tableColumn id="11" xr3:uid="{ACAFE223-634A-4220-89F7-A4378B0A4CB7}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{D4CFBB7D-1839-4E51-B405-B965D4BD5663}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{56759132-2838-427F-8CEB-7B84D96E48AD}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{763BB52C-9D74-4E50-8283-63C7653A623D}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{056D4100-CE19-456F-886C-346613E23F54}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{86C71EC7-589A-48F4-A94B-B0D31FE60863}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{B2834F24-112D-459F-B770-872CB2D2EA31}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{9ACC56B2-2F1F-47BE-AB93-DAFFAA80F3E3}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{BA39261E-2C8C-4139-B7E9-00D55BBF4287}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{AFEB0E62-F3EB-4854-B1CA-4A989BA06A87}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{22AF861C-2756-43B7-A352-3E30B03142CE}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{2044D69C-DD13-41EF-8B9B-60D8AEC112FB}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="3"/>
+    <tableColumn id="23" xr3:uid="{C74D06FB-AD56-4A98-983F-16DC10955D3B}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="2"/>
+    <tableColumn id="24" xr3:uid="{24D5DD84-F585-4F0A-AD0F-1604A8FD60A9}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5252,16 +5272,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698B00AE-22C7-4F47-B81E-0AD024323BD3}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>343</v>
       </c>
@@ -5280,7 +5301,7 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -5345,7 +5366,7 @@
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>105</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -5410,7 +5431,7 @@
       <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -5473,7 +5494,7 @@
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="3" t="s">
         <v>258</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -5536,7 +5557,7 @@
       <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>254</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -5599,7 +5620,7 @@
       <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="3" t="s">
         <v>251</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -5662,7 +5683,7 @@
       <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>248</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -5725,7 +5746,7 @@
       <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="3" t="s">
         <v>42</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -5788,7 +5809,7 @@
       <c r="F9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -5851,7 +5872,7 @@
       <c r="F10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>83</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -5914,7 +5935,7 @@
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -5977,7 +5998,7 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>262</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -6038,7 +6059,7 @@
       <c r="F13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -6099,7 +6120,7 @@
       <c r="F14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -6162,7 +6183,7 @@
       <c r="F15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="3" t="s">
         <v>267</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -6225,7 +6246,7 @@
       <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -6288,7 +6309,7 @@
       <c r="F17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>105</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -6351,7 +6372,7 @@
       <c r="F18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>114</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -6414,7 +6435,7 @@
       <c r="F19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="3" t="s">
         <v>67</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -6477,7 +6498,7 @@
       <c r="F20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" s="3" t="s">
         <v>274</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -6540,7 +6561,7 @@
       <c r="F21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="3" t="s">
         <v>281</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -6603,7 +6624,7 @@
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -6668,7 +6689,7 @@
       <c r="F23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -6733,7 +6754,7 @@
       <c r="F24" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="3" t="s">
         <v>73</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -6796,7 +6817,7 @@
       <c r="F25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="3" t="s">
         <v>291</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -6859,7 +6880,7 @@
       <c r="F26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="3" t="s">
         <v>296</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -6920,7 +6941,7 @@
       <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -6981,7 +7002,7 @@
       <c r="F28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="1" t="s">
+      <c r="G28" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -7042,7 +7063,7 @@
       <c r="F29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -7103,7 +7124,7 @@
       <c r="F30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="3" t="s">
         <v>73</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -7164,7 +7185,7 @@
       <c r="F31" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G31" s="1" t="s">
+      <c r="G31" s="3" t="s">
         <v>315</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -7225,7 +7246,7 @@
       <c r="F32" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -7286,7 +7307,7 @@
       <c r="F33" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -7347,7 +7368,7 @@
       <c r="F34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="3" t="s">
         <v>114</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -7408,7 +7429,7 @@
       <c r="F35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -7469,7 +7490,7 @@
       <c r="F36" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G36" s="1" t="s">
+      <c r="G36" s="3" t="s">
         <v>149</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -7530,7 +7551,7 @@
       <c r="F37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G37" s="3" t="s">
         <v>21</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -7591,7 +7612,7 @@
       <c r="F38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="3" t="s">
         <v>73</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -7652,7 +7673,7 @@
       <c r="F39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="3" t="s">
         <v>67</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -7713,7 +7734,7 @@
       <c r="F40" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="1" t="s">
+      <c r="G40" s="3" t="s">
         <v>114</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -7772,7 +7793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0340EF6C-49E5-4E36-B5BE-CFDD938CC6B0}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Arduino_r4wifi_matrix_gfx - complete update.
This no longer uses the Arduino_LED_Matrix library, but does all of its
work as self contained in this library.

It also adds support for setting how dim the pixels may be.  I have it setup for 4 colors.
</commit_message>
<xml_diff>
--- a/arduino_uno_r4.xlsx
+++ b/arduino_uno_r4.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\UNOR4-stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4813B8B-48C8-4633-B1B1-320544804825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ED7912-2E7D-48DA-AEF9-34560D14D6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5205" yWindow="630" windowWidth="24960" windowHeight="18450" activeTab="2" xr2:uid="{8DF1AF20-4F17-4E13-BB05-CAA1D9B0E58D}"/>
+    <workbookView xWindow="2340" yWindow="1395" windowWidth="27105" windowHeight="18450" activeTab="3" xr2:uid="{8DF1AF20-4F17-4E13-BB05-CAA1D9B0E58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Table033 (Page 23-26)" sheetId="2" r:id="rId1"/>
     <sheet name="Wifi" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Wifi-timer" sheetId="4" r:id="rId3"/>
     <sheet name="Minima" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">Minima!$C$1:$T$22</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">Minima!$B$1:$S$22</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Table033 (Page 23-26)'!$C$1:$T$53</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">Wifi!$D$1:$U$40</definedName>
   </definedNames>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2152" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="361">
   <si>
     <t>LQFP64</t>
   </si>
@@ -1212,12 +1212,24 @@
   <si>
     <t>Same Timer</t>
   </si>
+  <si>
+    <t>D0</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1227,13 +1239,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1253,7 +1258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1272,8 +1277,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1310,11 +1321,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1322,49 +1346,126 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="73">
     <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="11"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1525,6 +1626,31 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1546,93 +1672,6 @@
           <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1917,10 +1956,9 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="2" xr16:uid="{D2DECA6B-BF1E-43B8-9CD3-EAC049B0A48A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="28" unboundColumnsLeft="2">
-    <queryTableFields count="20">
+  <queryTableRefresh nextId="28" unboundColumnsLeft="1">
+    <queryTableFields count="19">
       <queryTableField id="26" dataBound="0" tableColumnId="25"/>
-      <queryTableField id="25" dataBound="0" tableColumnId="26"/>
       <queryTableField id="10" name="Column10" tableColumnId="10"/>
       <queryTableField id="3" name="Column3" tableColumnId="3"/>
       <queryTableField id="8" name="Column8" tableColumnId="8"/>
@@ -1953,115 +1991,114 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B50FC665-2B1E-4D36-B31E-B2C1FFAD1E63}" name="Table_Table033__Page_23_26" displayName="Table_Table033__Page_23_26" ref="A1:T53" tableType="queryTable" totalsRowShown="0" headerRowDxfId="73" dataDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B50FC665-2B1E-4D36-B31E-B2C1FFAD1E63}" name="Table_Table033__Page_23_26" displayName="Table_Table033__Page_23_26" ref="A1:T53" tableType="queryTable" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A1:T53" xr:uid="{B50FC665-2B1E-4D36-B31E-B2C1FFAD1E63}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T53">
     <sortCondition ref="B1:B53"/>
   </sortState>
   <tableColumns count="20">
-    <tableColumn id="25" xr3:uid="{A9DE5776-12F8-41C5-A53C-4CEA773E447C}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="71"/>
-    <tableColumn id="26" xr3:uid="{4A653EDD-EB22-4136-B683-155A497057BB}" uniqueName="26" name="WIFI" queryTableFieldId="25" dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{686632A6-7B4E-46CE-A17D-A61DACFEA311}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{F2F6AB26-F053-480A-8185-17F9C3A4E0E5}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="68"/>
-    <tableColumn id="8" xr3:uid="{64ADA7F2-5E91-4067-98B5-945EB7C4A19D}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="67"/>
-    <tableColumn id="9" xr3:uid="{2C66975A-6472-4704-A2BB-AFCE1DBA64F2}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{641C76F8-1FFC-4430-A657-32FB38B04E9A}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="65"/>
-    <tableColumn id="12" xr3:uid="{D1A66C96-F427-4AA0-B501-19F91F8C64FE}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="64"/>
-    <tableColumn id="13" xr3:uid="{26DD40DF-3192-44F9-B25D-8EFCA799F404}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="63"/>
-    <tableColumn id="14" xr3:uid="{111454D2-4353-4EB1-B9B3-DE3631B82E0E}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="62"/>
-    <tableColumn id="15" xr3:uid="{530DF3AC-0060-4870-8769-B78199F4FF48}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="61"/>
-    <tableColumn id="16" xr3:uid="{CFB946EF-B151-48CF-A6E8-0CD1CA40EAB1}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="60"/>
-    <tableColumn id="17" xr3:uid="{2095685C-F597-4A66-90B8-991C11FA59A9}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="59"/>
-    <tableColumn id="18" xr3:uid="{7738AAD1-7E59-4750-A6DA-F1491450160B}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="58"/>
-    <tableColumn id="19" xr3:uid="{6F4976C9-5965-4F43-A6D9-B6CE19B2DDA3}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="57"/>
-    <tableColumn id="20" xr3:uid="{0BCFC8CB-CEA6-4855-B4ED-7F154355114D}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="56"/>
-    <tableColumn id="21" xr3:uid="{5547BBC6-B268-4DF2-8784-C23E0E48A8EC}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="55"/>
-    <tableColumn id="22" xr3:uid="{7AEC012F-184E-49DA-8093-81B7FE607107}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="54"/>
-    <tableColumn id="23" xr3:uid="{C284EF91-8707-40FA-A12B-800FFB4C70C3}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="53"/>
-    <tableColumn id="24" xr3:uid="{4EC97FF2-42DA-4C41-B74D-F20F577DEE27}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="52"/>
+    <tableColumn id="25" xr3:uid="{A9DE5776-12F8-41C5-A53C-4CEA773E447C}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="70"/>
+    <tableColumn id="26" xr3:uid="{4A653EDD-EB22-4136-B683-155A497057BB}" uniqueName="26" name="WIFI" queryTableFieldId="25" dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{686632A6-7B4E-46CE-A17D-A61DACFEA311}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{F2F6AB26-F053-480A-8185-17F9C3A4E0E5}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{64ADA7F2-5E91-4067-98B5-945EB7C4A19D}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{2C66975A-6472-4704-A2BB-AFCE1DBA64F2}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="65"/>
+    <tableColumn id="11" xr3:uid="{641C76F8-1FFC-4430-A657-32FB38B04E9A}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="64"/>
+    <tableColumn id="12" xr3:uid="{D1A66C96-F427-4AA0-B501-19F91F8C64FE}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="63"/>
+    <tableColumn id="13" xr3:uid="{26DD40DF-3192-44F9-B25D-8EFCA799F404}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="62"/>
+    <tableColumn id="14" xr3:uid="{111454D2-4353-4EB1-B9B3-DE3631B82E0E}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="61"/>
+    <tableColumn id="15" xr3:uid="{530DF3AC-0060-4870-8769-B78199F4FF48}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="60"/>
+    <tableColumn id="16" xr3:uid="{CFB946EF-B151-48CF-A6E8-0CD1CA40EAB1}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="59"/>
+    <tableColumn id="17" xr3:uid="{2095685C-F597-4A66-90B8-991C11FA59A9}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="58"/>
+    <tableColumn id="18" xr3:uid="{7738AAD1-7E59-4750-A6DA-F1491450160B}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="57"/>
+    <tableColumn id="19" xr3:uid="{6F4976C9-5965-4F43-A6D9-B6CE19B2DDA3}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="56"/>
+    <tableColumn id="20" xr3:uid="{0BCFC8CB-CEA6-4855-B4ED-7F154355114D}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="55"/>
+    <tableColumn id="21" xr3:uid="{5547BBC6-B268-4DF2-8784-C23E0E48A8EC}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="54"/>
+    <tableColumn id="22" xr3:uid="{7AEC012F-184E-49DA-8093-81B7FE607107}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="53"/>
+    <tableColumn id="23" xr3:uid="{C284EF91-8707-40FA-A12B-800FFB4C70C3}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="52"/>
+    <tableColumn id="24" xr3:uid="{4EC97FF2-42DA-4C41-B74D-F20F577DEE27}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4C638A8D-F700-4C18-8C64-1A724FDCCFCB}" name="Table_Table033__Page_23_264" displayName="Table_Table033__Page_23_264" ref="A1:U40" tableType="queryTable" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4C638A8D-F700-4C18-8C64-1A724FDCCFCB}" name="Table_Table033__Page_23_264" displayName="Table_Table033__Page_23_264" ref="A1:U40" tableType="queryTable" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A1:U40" xr:uid="{4C638A8D-F700-4C18-8C64-1A724FDCCFCB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U40">
     <sortCondition ref="A1:A40"/>
   </sortState>
   <tableColumns count="21">
-    <tableColumn id="26" xr3:uid="{853CAB3E-22E9-47C9-9FDE-0C8F819ABB54}" uniqueName="26" name="WIFI" queryTableFieldId="25" dataDxfId="49"/>
-    <tableColumn id="27" xr3:uid="{0B1FA8E1-DA49-4FD0-9A12-8110E9B18983}" uniqueName="27" name="Main Usage" queryTableFieldId="29" dataDxfId="48"/>
-    <tableColumn id="25" xr3:uid="{443E811E-CB37-4948-8360-15EF75F1634E}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="47"/>
-    <tableColumn id="10" xr3:uid="{7CC39A3B-515E-4F8C-A6F7-2280B6C92DA1}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{A203754E-A450-4494-B6A5-44EF19BB1F8E}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="45"/>
-    <tableColumn id="8" xr3:uid="{4E09F24F-5659-4905-A86D-23D48584A50A}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="44"/>
-    <tableColumn id="9" xr3:uid="{EB3BAAA4-603C-40A6-9A4D-EC07A314AB5F}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{EB8A4512-2FDE-4FB0-B0DD-B6191ED09EEC}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{CF016CEA-ADC5-44A8-B471-E63CA06286F3}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{03E303EA-BF53-4F11-9DFA-1521FD43EB15}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="40"/>
-    <tableColumn id="14" xr3:uid="{C270C11F-4E2D-4E82-B1CC-0D68C3F1E880}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="39"/>
-    <tableColumn id="15" xr3:uid="{924B7926-CE59-4F31-AEED-2A32DF639D07}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="38"/>
-    <tableColumn id="16" xr3:uid="{F8FF5AAA-2E01-4762-A7A4-7E6F70376AAC}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="37"/>
-    <tableColumn id="17" xr3:uid="{D8E79A77-64C2-48C9-BB71-6D9C19FC3A1C}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="36"/>
-    <tableColumn id="18" xr3:uid="{C21D94B2-836A-4261-84CC-175D3F1E3353}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="35"/>
-    <tableColumn id="19" xr3:uid="{AC93E674-375E-4052-9969-9375BF1FD3A4}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="34"/>
-    <tableColumn id="20" xr3:uid="{B49C16CD-61A2-4F25-B45A-AFA4AAF0FC58}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="33"/>
-    <tableColumn id="21" xr3:uid="{D903978F-23DB-4B03-B7C9-BA809A44B21A}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="32"/>
-    <tableColumn id="22" xr3:uid="{81FBFEBF-D122-4513-86BC-F3847A1B490E}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="31"/>
-    <tableColumn id="23" xr3:uid="{14414913-AA39-4879-8F72-350C915855C1}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="30"/>
-    <tableColumn id="24" xr3:uid="{8CFBBC26-4A1C-44FE-BEDF-C020182C87C6}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="29"/>
+    <tableColumn id="26" xr3:uid="{853CAB3E-22E9-47C9-9FDE-0C8F819ABB54}" uniqueName="26" name="WIFI" queryTableFieldId="25" dataDxfId="48"/>
+    <tableColumn id="27" xr3:uid="{0B1FA8E1-DA49-4FD0-9A12-8110E9B18983}" uniqueName="27" name="Main Usage" queryTableFieldId="29" dataDxfId="47"/>
+    <tableColumn id="25" xr3:uid="{443E811E-CB37-4948-8360-15EF75F1634E}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="46"/>
+    <tableColumn id="10" xr3:uid="{7CC39A3B-515E-4F8C-A6F7-2280B6C92DA1}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{A203754E-A450-4494-B6A5-44EF19BB1F8E}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{4E09F24F-5659-4905-A86D-23D48584A50A}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="43"/>
+    <tableColumn id="9" xr3:uid="{EB3BAAA4-603C-40A6-9A4D-EC07A314AB5F}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{EB8A4512-2FDE-4FB0-B0DD-B6191ED09EEC}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="41"/>
+    <tableColumn id="12" xr3:uid="{CF016CEA-ADC5-44A8-B471-E63CA06286F3}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="40"/>
+    <tableColumn id="13" xr3:uid="{03E303EA-BF53-4F11-9DFA-1521FD43EB15}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="39"/>
+    <tableColumn id="14" xr3:uid="{C270C11F-4E2D-4E82-B1CC-0D68C3F1E880}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="38"/>
+    <tableColumn id="15" xr3:uid="{924B7926-CE59-4F31-AEED-2A32DF639D07}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="37"/>
+    <tableColumn id="16" xr3:uid="{F8FF5AAA-2E01-4762-A7A4-7E6F70376AAC}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="36"/>
+    <tableColumn id="17" xr3:uid="{D8E79A77-64C2-48C9-BB71-6D9C19FC3A1C}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="35"/>
+    <tableColumn id="18" xr3:uid="{C21D94B2-836A-4261-84CC-175D3F1E3353}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="34"/>
+    <tableColumn id="19" xr3:uid="{AC93E674-375E-4052-9969-9375BF1FD3A4}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="33"/>
+    <tableColumn id="20" xr3:uid="{B49C16CD-61A2-4F25-B45A-AFA4AAF0FC58}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="32"/>
+    <tableColumn id="21" xr3:uid="{D903978F-23DB-4B03-B7C9-BA809A44B21A}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="31"/>
+    <tableColumn id="22" xr3:uid="{81FBFEBF-D122-4513-86BC-F3847A1B490E}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="30"/>
+    <tableColumn id="23" xr3:uid="{14414913-AA39-4879-8F72-350C915855C1}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="29"/>
+    <tableColumn id="24" xr3:uid="{8CFBBC26-4A1C-44FE-BEDF-C020182C87C6}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="28"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3AFF5A15-7D47-46B8-B33F-177373666A65}" name="Table4" displayName="Table4" ref="A1:E17" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3AFF5A15-7D47-46B8-B33F-177373666A65}" name="Table4" displayName="Table4" ref="A1:E17" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
   <autoFilter ref="A1:E17" xr:uid="{3AFF5A15-7D47-46B8-B33F-177373666A65}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">
     <sortCondition ref="B2:B17"/>
     <sortCondition ref="A2:A17"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{BEC9DFF6-873D-458C-8A93-77A911B38A08}" name="WIFI" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{5C6802B3-0B1E-4BB1-B804-D60882C63F7E}" name="~" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{8370535D-8ABF-401A-8840-1AA8F1E9A320}" name="I/O ports" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{3E0F52DC-CCB6-4F54-A022-C5EDF480F244}" name="GPT" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{8680D23B-28E6-4D06-B248-E5E1BD2792EA}" name="Same Timer" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{BEC9DFF6-873D-458C-8A93-77A911B38A08}" name="WIFI" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{5C6802B3-0B1E-4BB1-B804-D60882C63F7E}" name="~" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{8370535D-8ABF-401A-8840-1AA8F1E9A320}" name="I/O ports" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{3E0F52DC-CCB6-4F54-A022-C5EDF480F244}" name="GPT" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{8680D23B-28E6-4D06-B248-E5E1BD2792EA}" name="Same Timer" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}" name="Table_Table033__Page_23_263" displayName="Table_Table033__Page_23_263" ref="A1:T22" tableType="queryTable" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A1:T22" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}" name="Table_Table033__Page_23_263" displayName="Table_Table033__Page_23_263" ref="A1:S22" tableType="queryTable" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S22" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S22">
     <sortCondition ref="A1:A22"/>
   </sortState>
-  <tableColumns count="20">
-    <tableColumn id="25" xr3:uid="{BE68D2CB-5447-4D49-B30A-0B4C0474174A}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="26"/>
-    <tableColumn id="26" xr3:uid="{84851A1F-0852-4293-AF8E-7CF07D757ECD}" uniqueName="26" name="WIFI" queryTableFieldId="25" dataDxfId="25"/>
-    <tableColumn id="10" xr3:uid="{2E3DDC90-3A23-41DD-AB0D-1BF738911004}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{82C193A7-9F71-4110-B199-955A18BF73C7}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{8C3AA304-F004-4A71-B050-8AA86784BA22}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{DAAC2DA6-CC15-480F-8376-08C7D49CCFAC}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{ACAFE223-634A-4220-89F7-A4378B0A4CB7}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{D4CFBB7D-1839-4E51-B405-B965D4BD5663}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="19"/>
-    <tableColumn id="13" xr3:uid="{56759132-2838-427F-8CEB-7B84D96E48AD}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{763BB52C-9D74-4E50-8283-63C7653A623D}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="17"/>
-    <tableColumn id="15" xr3:uid="{056D4100-CE19-456F-886C-346613E23F54}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="16"/>
-    <tableColumn id="16" xr3:uid="{86C71EC7-589A-48F4-A94B-B0D31FE60863}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="15"/>
-    <tableColumn id="17" xr3:uid="{B2834F24-112D-459F-B770-872CB2D2EA31}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="14"/>
-    <tableColumn id="18" xr3:uid="{9ACC56B2-2F1F-47BE-AB93-DAFFAA80F3E3}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="13"/>
-    <tableColumn id="19" xr3:uid="{BA39261E-2C8C-4139-B7E9-00D55BBF4287}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{AFEB0E62-F3EB-4854-B1CA-4A989BA06A87}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{22AF861C-2756-43B7-A352-3E30B03142CE}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{2044D69C-DD13-41EF-8B9B-60D8AEC112FB}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="9"/>
-    <tableColumn id="23" xr3:uid="{C74D06FB-AD56-4A98-983F-16DC10955D3B}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="8"/>
-    <tableColumn id="24" xr3:uid="{24D5DD84-F585-4F0A-AD0F-1604A8FD60A9}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="7"/>
+  <tableColumns count="19">
+    <tableColumn id="25" xr3:uid="{BE68D2CB-5447-4D49-B30A-0B4C0474174A}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{2E3DDC90-3A23-41DD-AB0D-1BF738911004}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{82C193A7-9F71-4110-B199-955A18BF73C7}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{8C3AA304-F004-4A71-B050-8AA86784BA22}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{DAAC2DA6-CC15-480F-8376-08C7D49CCFAC}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{ACAFE223-634A-4220-89F7-A4378B0A4CB7}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="14"/>
+    <tableColumn id="12" xr3:uid="{D4CFBB7D-1839-4E51-B405-B965D4BD5663}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{56759132-2838-427F-8CEB-7B84D96E48AD}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{763BB52C-9D74-4E50-8283-63C7653A623D}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{056D4100-CE19-456F-886C-346613E23F54}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="10"/>
+    <tableColumn id="16" xr3:uid="{86C71EC7-589A-48F4-A94B-B0D31FE60863}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="9"/>
+    <tableColumn id="17" xr3:uid="{B2834F24-112D-459F-B770-872CB2D2EA31}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="8"/>
+    <tableColumn id="18" xr3:uid="{9ACC56B2-2F1F-47BE-AB93-DAFFAA80F3E3}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{BA39261E-2C8C-4139-B7E9-00D55BBF4287}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="6"/>
+    <tableColumn id="20" xr3:uid="{AFEB0E62-F3EB-4854-B1CA-4A989BA06A87}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="5"/>
+    <tableColumn id="21" xr3:uid="{22AF861C-2756-43B7-A352-3E30B03142CE}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="4"/>
+    <tableColumn id="22" xr3:uid="{2044D69C-DD13-41EF-8B9B-60D8AEC112FB}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="3"/>
+    <tableColumn id="23" xr3:uid="{C74D06FB-AD56-4A98-983F-16DC10955D3B}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="2"/>
+    <tableColumn id="24" xr3:uid="{24D5DD84-F585-4F0A-AD0F-1604A8FD60A9}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5563,14 +5600,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698B00AE-22C7-4F47-B81E-0AD024323BD3}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
     <col min="10" max="10" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5593,7 +5630,7 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -5658,7 +5695,7 @@
       <c r="F2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -5723,7 +5760,7 @@
       <c r="F3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H3" s="1" t="s">
@@ -5786,7 +5823,7 @@
       <c r="F4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>258</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -5849,7 +5886,7 @@
       <c r="F5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>254</v>
       </c>
       <c r="H5" s="1" t="s">
@@ -5912,7 +5949,7 @@
       <c r="F6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>251</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -5975,7 +6012,7 @@
       <c r="F7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>248</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -6038,7 +6075,7 @@
       <c r="F8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -6101,7 +6138,7 @@
       <c r="F9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -6164,7 +6201,7 @@
       <c r="F10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>83</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -6227,7 +6264,7 @@
       <c r="F11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -6290,7 +6327,7 @@
       <c r="F12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>262</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -6351,7 +6388,7 @@
       <c r="F13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -6412,7 +6449,7 @@
       <c r="F14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -6475,7 +6512,7 @@
       <c r="F15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>267</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -6538,7 +6575,7 @@
       <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H16" s="1" t="s">
@@ -6601,7 +6638,7 @@
       <c r="F17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>105</v>
       </c>
       <c r="H17" s="1" t="s">
@@ -6664,7 +6701,7 @@
       <c r="F18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>114</v>
       </c>
       <c r="H18" s="1" t="s">
@@ -6727,7 +6764,7 @@
       <c r="F19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>67</v>
       </c>
       <c r="H19" s="1" t="s">
@@ -6790,7 +6827,7 @@
       <c r="F20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>274</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -6853,7 +6890,7 @@
       <c r="F21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>281</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -6916,7 +6953,7 @@
       <c r="F22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -6981,7 +7018,7 @@
       <c r="F23" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="1" t="s">
@@ -7046,7 +7083,7 @@
       <c r="F24" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G24" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -7109,7 +7146,7 @@
       <c r="F25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="3" t="s">
+      <c r="G25" s="2" t="s">
         <v>291</v>
       </c>
       <c r="H25" s="1" t="s">
@@ -7172,7 +7209,7 @@
       <c r="F26" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G26" s="3" t="s">
+      <c r="G26" s="2" t="s">
         <v>296</v>
       </c>
       <c r="H26" s="1" t="s">
@@ -7233,7 +7270,7 @@
       <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="G27" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -7294,7 +7331,7 @@
       <c r="F28" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="H28" s="1" t="s">
@@ -7355,7 +7392,7 @@
       <c r="F29" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G29" s="3" t="s">
+      <c r="G29" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H29" s="1" t="s">
@@ -7416,7 +7453,7 @@
       <c r="F30" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G30" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H30" s="1" t="s">
@@ -7477,7 +7514,7 @@
       <c r="F31" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="2" t="s">
         <v>315</v>
       </c>
       <c r="H31" s="1" t="s">
@@ -7538,7 +7575,7 @@
       <c r="F32" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="G32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H32" s="1" t="s">
@@ -7599,7 +7636,7 @@
       <c r="F33" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="G33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H33" s="1" t="s">
@@ -7660,7 +7697,7 @@
       <c r="F34" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>114</v>
       </c>
       <c r="H34" s="1" t="s">
@@ -7721,7 +7758,7 @@
       <c r="F35" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G35" s="3" t="s">
+      <c r="G35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="H35" s="1" t="s">
@@ -7782,7 +7819,7 @@
       <c r="F36" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="G36" s="3" t="s">
+      <c r="G36" s="2" t="s">
         <v>149</v>
       </c>
       <c r="H36" s="1" t="s">
@@ -7843,7 +7880,7 @@
       <c r="F37" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G37" s="3" t="s">
+      <c r="G37" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H37" s="1" t="s">
@@ -7904,7 +7941,7 @@
       <c r="F38" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>73</v>
       </c>
       <c r="H38" s="1" t="s">
@@ -7965,7 +8002,7 @@
       <c r="F39" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G39" s="3" t="s">
+      <c r="G39" s="2" t="s">
         <v>67</v>
       </c>
       <c r="H39" s="1" t="s">
@@ -8026,7 +8063,7 @@
       <c r="F40" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="G40" s="2" t="s">
         <v>114</v>
       </c>
       <c r="H40" s="1" t="s">
@@ -8083,10 +8120,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E61DAF-7D47-4EBC-815E-8385629E20B2}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8096,272 +8133,332 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>9</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>10</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>11</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>0</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>1</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>2</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>4</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>7</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12">
         <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>8</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>12</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>13</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>18</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16">
         <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>19</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9" t="s">
+      <c r="A17" s="7">
+        <v>19</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17">
         <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>34</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E19" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>35</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>37</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>38</v>
+      </c>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -8377,118 +8474,118 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0340EF6C-49E5-4E36-B5BE-CFDD938CC6B0}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>342</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>343</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
-        <v>0</v>
+      <c r="B2" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>202</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>123</v>
+        <v>203</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>163</v>
+        <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>19</v>
+        <v>204</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>204</v>
+        <v>19</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>19</v>
+        <v>205</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>205</v>
+        <v>19</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>19</v>
@@ -8500,57 +8597,54 @@
         <v>19</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>19</v>
+        <v>206</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="T2" s="1" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
+      <c r="B3" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>196</v>
+        <v>138</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>197</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>153</v>
+        <v>19</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>19</v>
+        <v>198</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>198</v>
+        <v>19</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>19</v>
+        <v>126</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>126</v>
+        <v>19</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>19</v>
@@ -8562,42 +8656,39 @@
         <v>19</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>19</v>
+        <v>199</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="T3" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
-        <v>3</v>
+      <c r="B4" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>255</v>
+        <v>182</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>254</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G4" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>19</v>
@@ -8609,10 +8700,10 @@
         <v>19</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>81</v>
+        <v>19</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>19</v>
@@ -8624,57 +8715,54 @@
         <v>19</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>19</v>
+        <v>256</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="T4" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
-        <v>2</v>
+      <c r="B5" s="1" t="s">
+        <v>259</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>259</v>
+        <v>183</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>258</v>
       </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G5" s="1" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>19</v>
@@ -8686,166 +8774,157 @@
         <v>19</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>19</v>
+        <v>260</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="T5" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
-        <v>10</v>
+      <c r="B6" s="1" t="s">
+        <v>263</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>263</v>
+        <v>188</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>262</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>262</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>19</v>
+        <v>107</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>107</v>
+        <v>237</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>237</v>
+        <v>19</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>87</v>
+        <v>19</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>19</v>
+        <v>264</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>264</v>
+        <v>19</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>19</v>
+        <v>265</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="T6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
-        <v>13</v>
+      <c r="B7" s="1" t="s">
+        <v>268</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>268</v>
+        <v>189</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>267</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>269</v>
+        <v>116</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>116</v>
+        <v>240</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>240</v>
+        <v>19</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>46</v>
+        <v>270</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>270</v>
+        <v>19</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>19</v>
+        <v>271</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>271</v>
+        <v>19</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>19</v>
+        <v>272</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="T7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
-        <v>4</v>
+      <c r="B8" s="1" t="s">
+        <v>252</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>252</v>
+        <v>181</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>251</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>251</v>
+        <v>19</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>19</v>
+        <v>77</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>19</v>
@@ -8857,10 +8936,10 @@
         <v>19</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>80</v>
+        <v>19</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>19</v>
@@ -8872,42 +8951,39 @@
         <v>19</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>19</v>
+        <v>253</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
-        <v>5</v>
+      <c r="B9" s="1" t="s">
+        <v>249</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>249</v>
+        <v>180</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>248</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>248</v>
+        <v>19</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>19</v>
@@ -8934,42 +9010,39 @@
         <v>19</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>19</v>
+        <v>250</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
-        <v>8</v>
+      <c r="B10" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>19</v>
+        <v>185</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>185</v>
+        <v>19</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>19</v>
@@ -8996,29 +9069,26 @@
         <v>19</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>19</v>
+        <v>186</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="T10" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
-        <v>9</v>
+      <c r="B11" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>191</v>
+        <v>137</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -9028,10 +9098,10 @@
         <v>19</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>19</v>
+        <v>192</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>192</v>
+        <v>19</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>19</v>
@@ -9058,29 +9128,26 @@
         <v>19</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>19</v>
+        <v>193</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="T11" s="1" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
-        <v>7</v>
+      <c r="B12" s="1" t="s">
+        <v>233</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>233</v>
+        <v>174</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="E12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -9090,28 +9157,28 @@
         <v>19</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>19</v>
+        <v>234</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>234</v>
+        <v>19</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>19</v>
+        <v>157</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>157</v>
+        <v>51</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
       <c r="P12" s="1" t="s">
         <v>19</v>
@@ -9120,57 +9187,54 @@
         <v>19</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>19</v>
+        <v>235</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="T12" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
-        <v>22</v>
+      <c r="B13" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>217</v>
+        <v>169</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E13" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>55</v>
+        <v>19</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>35</v>
+        <v>218</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>218</v>
+        <v>19</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>19</v>
+        <v>170</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>170</v>
+        <v>19</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>19</v>
@@ -9182,57 +9246,54 @@
         <v>19</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>19</v>
+        <v>219</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="T13" s="1" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
-        <v>23</v>
+      <c r="B14" s="1" t="s">
+        <v>223</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>223</v>
+        <v>171</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E14" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G14" s="1" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>46</v>
+        <v>224</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>224</v>
+        <v>19</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>19</v>
+        <v>172</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>172</v>
+        <v>19</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>19</v>
@@ -9241,60 +9302,57 @@
         <v>19</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>19</v>
+        <v>225</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="T14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
-        <v>6</v>
+      <c r="B15" s="1" t="s">
+        <v>228</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="F15" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>19</v>
+        <v>229</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>229</v>
+        <v>19</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>19</v>
+        <v>166</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>166</v>
+        <v>19</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>19</v>
@@ -9306,29 +9364,26 @@
         <v>19</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>19</v>
+        <v>230</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="T15" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>344</v>
+        <v>303</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>303</v>
+        <v>221</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="E16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -9359,13 +9414,13 @@
         <v>19</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>19</v>
+        <v>304</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>305</v>
+        <v>19</v>
       </c>
       <c r="R16" s="1" t="s">
         <v>19</v>
@@ -9373,29 +9428,26 @@
       <c r="S16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>338</v>
+        <v>247</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="F17" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G17" s="1" t="s">
         <v>19</v>
       </c>
@@ -9421,43 +9473,40 @@
         <v>19</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>19</v>
+        <v>339</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>340</v>
+        <v>19</v>
       </c>
       <c r="R17" s="1" t="s">
         <v>19</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T17" s="1" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>334</v>
+        <v>246</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>114</v>
       </c>
+      <c r="F18" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G18" s="1" t="s">
         <v>19</v>
       </c>
@@ -9483,43 +9532,40 @@
         <v>19</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>19</v>
+        <v>335</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>336</v>
+        <v>19</v>
       </c>
       <c r="R18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T18" s="1" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>331</v>
+        <v>245</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="F19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G19" s="1" t="s">
         <v>19</v>
       </c>
@@ -9545,13 +9591,13 @@
         <v>19</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>19</v>
+        <v>332</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>333</v>
+        <v>19</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>19</v>
@@ -9559,167 +9605,158 @@
       <c r="S19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:19" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>348</v>
+        <v>275</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>275</v>
+        <v>190</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>274</v>
       </c>
+      <c r="F20" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="G20" s="1" t="s">
-        <v>276</v>
+        <v>76</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>108</v>
+        <v>19</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>19</v>
+        <v>277</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>277</v>
+        <v>143</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>19</v>
+        <v>278</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>278</v>
+        <v>19</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>19</v>
+        <v>279</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="T20" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>349</v>
+        <v>282</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>282</v>
+        <v>195</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>281</v>
       </c>
+      <c r="F21" s="1" t="s">
+        <v>123</v>
+      </c>
       <c r="G21" s="1" t="s">
-        <v>123</v>
+        <v>33</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>19</v>
+        <v>283</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>283</v>
+        <v>156</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>156</v>
+        <v>101</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>101</v>
+        <v>19</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>19</v>
+        <v>284</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>284</v>
+        <v>19</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>19</v>
+        <v>285</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="1">
-        <v>20</v>
+      <c r="B22" s="1" t="s">
+        <v>287</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>287</v>
+        <v>201</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>19</v>
+        <v>288</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>288</v>
+        <v>141</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>141</v>
+        <v>237</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>237</v>
+        <v>19</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="L22" s="1" t="s">
         <v>19</v>
@@ -9731,21 +9768,18 @@
         <v>19</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>19</v>
+        <v>289</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>289</v>
+        <v>19</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>19</v>
+        <v>265</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>265</v>
+        <v>290</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="T22" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new MINIMA pin defines to table
</commit_message>
<xml_diff>
--- a/arduino_uno_r4.xlsx
+++ b/arduino_uno_r4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\UNOR4-stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ED7912-2E7D-48DA-AEF9-34560D14D6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF20782F-896D-49E7-B65D-C942F1D8B7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1395" windowWidth="27105" windowHeight="18450" activeTab="3" xr2:uid="{8DF1AF20-4F17-4E13-BB05-CAA1D9B0E58D}"/>
+    <workbookView xWindow="2250" yWindow="2190" windowWidth="20310" windowHeight="16950" activeTab="3" xr2:uid="{8DF1AF20-4F17-4E13-BB05-CAA1D9B0E58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Table033 (Page 23-26)" sheetId="2" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="Minima" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="3" hidden="1">Minima!$B$1:$S$22</definedName>
+    <definedName name="ExternalData_1" localSheetId="3" hidden="1">Minima!$B$1:$S$28</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Table033 (Page 23-26)'!$C$1:$T$53</definedName>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Wifi!$D$1:$U$40</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Wifi!$A$1:$U$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2157" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2221" uniqueCount="386">
   <si>
     <t>LQFP64</t>
   </si>
@@ -1223,6 +1223,81 @@
   </si>
   <si>
     <t>D5</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>D3~</t>
+  </si>
+  <si>
+    <t>D5~</t>
+  </si>
+  <si>
+    <t>D6~</t>
+  </si>
+  <si>
+    <t>D9~</t>
+  </si>
+  <si>
+    <t>D10~</t>
+  </si>
+  <si>
+    <t>D11~</t>
+  </si>
+  <si>
+    <t>A4/SDA</t>
+  </si>
+  <si>
+    <t>A5/SCL</t>
+  </si>
+  <si>
+    <t>Analog voltage measure</t>
+  </si>
+  <si>
+    <t>TX LED</t>
+  </si>
+  <si>
+    <t>RX LED</t>
+  </si>
+  <si>
+    <t>TX on SWD(8)</t>
+  </si>
+  <si>
+    <t>RX on SWD(7)</t>
+  </si>
+  <si>
+    <t>SWDIO on SWD(2)</t>
+  </si>
+  <si>
+    <t>SWCLK on SWD(4)</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1366,26 +1441,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="73">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1442,6 +1509,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2074,31 +2155,31 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}" name="Table_Table033__Page_23_263" displayName="Table_Table033__Page_23_263" ref="A1:S22" tableType="queryTable" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:S22" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}" name="Table_Table033__Page_23_263" displayName="Table_Table033__Page_23_263" ref="A1:S28" tableType="queryTable" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A1:S28" xr:uid="{7487EA7B-3A33-4420-8CFE-36E1C2A9C8E4}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S22">
     <sortCondition ref="A1:A22"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="25" xr3:uid="{BE68D2CB-5447-4D49-B30A-0B4C0474174A}" uniqueName="25" name="Minima" queryTableFieldId="26" dataDxfId="18"/>
     <tableColumn id="10" xr3:uid="{2E3DDC90-3A23-41DD-AB0D-1BF738911004}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{82C193A7-9F71-4110-B199-955A18BF73C7}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{82C193A7-9F71-4110-B199-955A18BF73C7}" uniqueName="3" name="Usage" queryTableFieldId="3" dataDxfId="16"/>
     <tableColumn id="8" xr3:uid="{8C3AA304-F004-4A71-B050-8AA86784BA22}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{DAAC2DA6-CC15-480F-8376-08C7D49CCFAC}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{ACAFE223-634A-4220-89F7-A4378B0A4CB7}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{D4CFBB7D-1839-4E51-B405-B965D4BD5663}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{56759132-2838-427F-8CEB-7B84D96E48AD}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{763BB52C-9D74-4E50-8283-63C7653A623D}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{056D4100-CE19-456F-886C-346613E23F54}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{86C71EC7-589A-48F4-A94B-B0D31FE60863}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{B2834F24-112D-459F-B770-872CB2D2EA31}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{9ACC56B2-2F1F-47BE-AB93-DAFFAA80F3E3}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{BA39261E-2C8C-4139-B7E9-00D55BBF4287}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{AFEB0E62-F3EB-4854-B1CA-4A989BA06A87}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{22AF861C-2756-43B7-A352-3E30B03142CE}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{2044D69C-DD13-41EF-8B9B-60D8AEC112FB}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="3"/>
-    <tableColumn id="23" xr3:uid="{C74D06FB-AD56-4A98-983F-16DC10955D3B}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="2"/>
-    <tableColumn id="24" xr3:uid="{24D5DD84-F585-4F0A-AD0F-1604A8FD60A9}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{DAAC2DA6-CC15-480F-8376-08C7D49CCFAC}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{ACAFE223-634A-4220-89F7-A4378B0A4CB7}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{D4CFBB7D-1839-4E51-B405-B965D4BD5663}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{56759132-2838-427F-8CEB-7B84D96E48AD}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{763BB52C-9D74-4E50-8283-63C7653A623D}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{056D4100-CE19-456F-886C-346613E23F54}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{86C71EC7-589A-48F4-A94B-B0D31FE60863}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{B2834F24-112D-459F-B770-872CB2D2EA31}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{9ACC56B2-2F1F-47BE-AB93-DAFFAA80F3E3}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{BA39261E-2C8C-4139-B7E9-00D55BBF4287}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{AFEB0E62-F3EB-4854-B1CA-4A989BA06A87}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{22AF861C-2756-43B7-A352-3E30B03142CE}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{2044D69C-DD13-41EF-8B9B-60D8AEC112FB}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{C74D06FB-AD56-4A98-983F-16DC10955D3B}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{24D5DD84-F585-4F0A-AD0F-1604A8FD60A9}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2404,7 +2485,7 @@
   <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:T53"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5600,8 +5681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698B00AE-22C7-4F47-B81E-0AD024323BD3}">
   <dimension ref="A1:U40"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6999,194 +7080,192 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+    <row r="23" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>22</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="C23" s="1">
-        <v>11</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L23" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M23" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T23" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="U23" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>353</v>
       </c>
       <c r="C24" s="1">
+        <v>11</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C25" s="1">
         <v>12</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D25" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="H25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L24" s="1" t="s">
+      <c r="K25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="M25" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O24" s="1" t="s">
+      <c r="N25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O25" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S24" s="1" t="s">
+      <c r="P25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S25" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="T24" s="1" t="s">
+      <c r="T25" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q25" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="R25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S25" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="T25" s="1" t="s">
-        <v>295</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>19</v>
@@ -7194,41 +7273,41 @@
     </row>
     <row r="26" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>354</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>19</v>
+        <v>293</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>52</v>
+        <v>240</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="M26" s="1" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>19</v>
@@ -7240,16 +7319,16 @@
         <v>19</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="R26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="U26" s="1" t="s">
         <v>19</v>
@@ -7257,109 +7336,111 @@
     </row>
     <row r="27" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1" t="s">
-        <v>22</v>
+        <v>297</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>211</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>21</v>
+        <v>296</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>19</v>
+        <v>162</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="N27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
         <v>26</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="R27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="U27" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>19</v>
@@ -7371,50 +7452,50 @@
         <v>19</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1" t="s">
-        <v>328</v>
+        <v>32</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>244</v>
+        <v>30</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="O29" s="1" t="s">
         <v>19</v>
@@ -7423,38 +7504,38 @@
         <v>19</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>329</v>
+        <v>19</v>
       </c>
       <c r="R29" s="1" t="s">
-        <v>330</v>
+        <v>19</v>
       </c>
       <c r="S29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="T29" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>19</v>
@@ -7484,10 +7565,10 @@
         <v>19</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="S30" s="1" t="s">
         <v>19</v>
@@ -7501,21 +7582,21 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>314</v>
+        <v>19</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>315</v>
+        <v>73</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>19</v>
@@ -7545,10 +7626,10 @@
         <v>19</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="R31" s="1" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="S31" s="1" t="s">
         <v>19</v>
@@ -7557,26 +7638,26 @@
         <v>19</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>319</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>19</v>
+        <v>315</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>19</v>
@@ -7606,10 +7687,10 @@
         <v>19</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="R32" s="1" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="S32" s="1" t="s">
         <v>19</v>
@@ -7618,23 +7699,23 @@
         <v>19</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>19</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>19</v>
@@ -7667,10 +7748,10 @@
         <v>19</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="R33" s="1" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="S33" s="1" t="s">
         <v>19</v>
@@ -7684,21 +7765,21 @@
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>19</v>
+        <v>306</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>114</v>
+        <v>19</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>19</v>
@@ -7728,10 +7809,10 @@
         <v>19</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="R34" s="1" t="s">
-        <v>19</v>
+        <v>309</v>
       </c>
       <c r="S34" s="1" t="s">
         <v>19</v>
@@ -7740,56 +7821,56 @@
         <v>19</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1" t="s">
-        <v>161</v>
+        <v>300</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>19</v>
+        <v>114</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>162</v>
+        <v>19</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>163</v>
+        <v>19</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>164</v>
+        <v>19</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>165</v>
+        <v>19</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>166</v>
+        <v>19</v>
       </c>
       <c r="P35" s="1" t="s">
         <v>19</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>19</v>
+        <v>301</v>
       </c>
       <c r="R35" s="1" t="s">
         <v>19</v>
@@ -7798,53 +7879,53 @@
         <v>19</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>167</v>
+        <v>19</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="90" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>148</v>
+        <v>20</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>149</v>
+        <v>19</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="P36" s="1" t="s">
         <v>19</v>
@@ -7859,53 +7940,53 @@
         <v>19</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="90" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>19</v>
+        <v>148</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>21</v>
+        <v>149</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>19</v>
+        <v>153</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="M37" s="1" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="P37" s="1" t="s">
         <v>19</v>
@@ -7920,53 +8001,53 @@
         <v>19</v>
       </c>
       <c r="T37" s="1" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>75</v>
+        <v>19</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>77</v>
+        <v>19</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="M38" s="1" t="s">
-        <v>47</v>
+        <v>100</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>19</v>
+        <v>143</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>19</v>
+        <v>144</v>
       </c>
       <c r="P38" s="1" t="s">
         <v>19</v>
@@ -7981,38 +8062,38 @@
         <v>19</v>
       </c>
       <c r="T38" s="1" t="s">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>19</v>
@@ -8021,7 +8102,7 @@
         <v>19</v>
       </c>
       <c r="M39" s="1" t="s">
-        <v>70</v>
+        <v>47</v>
       </c>
       <c r="N39" s="1" t="s">
         <v>19</v>
@@ -8048,44 +8129,44 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:21" ht="90" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>350</v>
+    <row r="40" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1" t="s">
-        <v>115</v>
+        <v>68</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>114</v>
+        <v>67</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>116</v>
+        <v>33</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>118</v>
+        <v>19</v>
       </c>
       <c r="M40" s="1" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="O40" s="1" t="s">
         <v>19</v>
@@ -8103,10 +8184,10 @@
         <v>19</v>
       </c>
       <c r="T40" s="1" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>121</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -8474,10 +8555,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0340EF6C-49E5-4E36-B5BE-CFDD938CC6B0}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8493,7 +8575,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>361</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -8552,7 +8634,7 @@
         <v>202</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>139</v>
+        <v>357</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -8611,7 +8693,7 @@
         <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>138</v>
+        <v>358</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>19</v>
@@ -8670,7 +8752,7 @@
         <v>255</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>182</v>
+        <v>362</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -8729,7 +8811,7 @@
         <v>259</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>183</v>
+        <v>371</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>19</v>
@@ -8788,7 +8870,7 @@
         <v>263</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>188</v>
+        <v>359</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>19</v>
@@ -8847,7 +8929,7 @@
         <v>268</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>189</v>
+        <v>372</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>19</v>
@@ -8906,7 +8988,7 @@
         <v>252</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>181</v>
+        <v>373</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>19</v>
@@ -8965,7 +9047,7 @@
         <v>249</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>180</v>
+        <v>363</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>19</v>
@@ -9024,7 +9106,7 @@
         <v>184</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>134</v>
+        <v>364</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>19</v>
@@ -9083,7 +9165,7 @@
         <v>191</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>137</v>
+        <v>374</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>19</v>
@@ -9142,7 +9224,7 @@
         <v>233</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>174</v>
+        <v>375</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>19</v>
@@ -9201,7 +9283,7 @@
         <v>217</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>169</v>
+        <v>376</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>216</v>
@@ -9260,7 +9342,7 @@
         <v>223</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>171</v>
+        <v>365</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>222</v>
@@ -9319,7 +9401,7 @@
         <v>228</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>173</v>
+        <v>366</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>19</v>
@@ -9378,7 +9460,7 @@
         <v>303</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>221</v>
+        <v>367</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>19</v>
@@ -9437,7 +9519,7 @@
         <v>338</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>247</v>
+        <v>368</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>19</v>
@@ -9496,7 +9578,7 @@
         <v>334</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>246</v>
+        <v>369</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
@@ -9555,7 +9637,7 @@
         <v>331</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>245</v>
+        <v>370</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
@@ -9614,7 +9696,7 @@
         <v>275</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>190</v>
+        <v>377</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>19</v>
@@ -9673,7 +9755,7 @@
         <v>282</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>195</v>
+        <v>378</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>19</v>
@@ -9732,7 +9814,7 @@
         <v>287</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>201</v>
+        <v>379</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>19</v>
@@ -9782,6 +9864,270 @@
       <c r="S22" s="1" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>21</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="S23" s="11"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>22</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>307</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="11"/>
+    </row>
+    <row r="25" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>23</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>292</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="S25" s="11"/>
+    </row>
+    <row r="26" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>24</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>297</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="S26" s="11"/>
+    </row>
+    <row r="27" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>25</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="L27" s="11"/>
+      <c r="M27" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="11"/>
+      <c r="S27" s="11"/>
+    </row>
+    <row r="28" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>26</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>385</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
synchronize what I have
</commit_message>
<xml_diff>
--- a/arduino_uno_r4.xlsx
+++ b/arduino_uno_r4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\UNOR4-stuff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4ED7912-2E7D-48DA-AEF9-34560D14D6C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4997D2B-A068-4648-B657-4735A902C82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1395" windowWidth="27105" windowHeight="18450" activeTab="3" xr2:uid="{8DF1AF20-4F17-4E13-BB05-CAA1D9B0E58D}"/>
+    <workbookView xWindow="840" yWindow="2745" windowWidth="19845" windowHeight="14340" activeTab="3" xr2:uid="{8DF1AF20-4F17-4E13-BB05-CAA1D9B0E58D}"/>
   </bookViews>
   <sheets>
     <sheet name="Table033 (Page 23-26)" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">Wifi!$D$1:$U$40</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1372,20 +1373,6 @@
   </cellStyles>
   <dxfs count="73">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1442,6 +1429,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2084,30 +2085,30 @@
     <tableColumn id="10" xr3:uid="{2E3DDC90-3A23-41DD-AB0D-1BF738911004}" uniqueName="10" name="I/O ports" queryTableFieldId="10" dataDxfId="17"/>
     <tableColumn id="3" xr3:uid="{82C193A7-9F71-4110-B199-955A18BF73C7}" uniqueName="3" name="LQFP64" queryTableFieldId="3" dataDxfId="16"/>
     <tableColumn id="8" xr3:uid="{8C3AA304-F004-4A71-B050-8AA86784BA22}" uniqueName="8" name="Power, System, Clock,_x000a_Debug, CAC, VBATT" queryTableFieldId="8" dataDxfId="15"/>
-    <tableColumn id="9" xr3:uid="{DAAC2DA6-CC15-480F-8376-08C7D49CCFAC}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{ACAFE223-634A-4220-89F7-A4378B0A4CB7}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{D4CFBB7D-1839-4E51-B405-B965D4BD5663}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{56759132-2838-427F-8CEB-7B84D96E48AD}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{763BB52C-9D74-4E50-8283-63C7653A623D}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{056D4100-CE19-456F-886C-346613E23F54}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{86C71EC7-589A-48F4-A94B-B0D31FE60863}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{B2834F24-112D-459F-B770-872CB2D2EA31}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{9ACC56B2-2F1F-47BE-AB93-DAFFAA80F3E3}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{BA39261E-2C8C-4139-B7E9-00D55BBF4287}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{AFEB0E62-F3EB-4854-B1CA-4A989BA06A87}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{22AF861C-2756-43B7-A352-3E30B03142CE}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{2044D69C-DD13-41EF-8B9B-60D8AEC112FB}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="3"/>
-    <tableColumn id="23" xr3:uid="{C74D06FB-AD56-4A98-983F-16DC10955D3B}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="2"/>
-    <tableColumn id="24" xr3:uid="{24D5DD84-F585-4F0A-AD0F-1604A8FD60A9}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{DAAC2DA6-CC15-480F-8376-08C7D49CCFAC}" uniqueName="9" name="Interrupt" queryTableFieldId="9" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{ACAFE223-634A-4220-89F7-A4378B0A4CB7}" uniqueName="11" name="AGT" queryTableFieldId="11" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{D4CFBB7D-1839-4E51-B405-B965D4BD5663}" uniqueName="12" name="GPT_OPS, POEG" queryTableFieldId="12" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{56759132-2838-427F-8CEB-7B84D96E48AD}" uniqueName="13" name="GPT" queryTableFieldId="13" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{763BB52C-9D74-4E50-8283-63C7653A623D}" uniqueName="14" name="RTC" queryTableFieldId="14" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{056D4100-CE19-456F-886C-346613E23F54}" uniqueName="15" name="USBFS,CAN" queryTableFieldId="15" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{86C71EC7-589A-48F4-A94B-B0D31FE60863}" uniqueName="16" name="SCI" queryTableFieldId="16" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{B2834F24-112D-459F-B770-872CB2D2EA31}" uniqueName="17" name="IIC" queryTableFieldId="17" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{9ACC56B2-2F1F-47BE-AB93-DAFFAA80F3E3}" uniqueName="18" name="SPI" queryTableFieldId="18" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{BA39261E-2C8C-4139-B7E9-00D55BBF4287}" uniqueName="19" name="SSIE" queryTableFieldId="19" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{AFEB0E62-F3EB-4854-B1CA-4A989BA06A87}" uniqueName="20" name="ADC14" queryTableFieldId="20" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{22AF861C-2756-43B7-A352-3E30B03142CE}" uniqueName="21" name="DAC12, OPAMP" queryTableFieldId="21" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{2044D69C-DD13-41EF-8B9B-60D8AEC112FB}" uniqueName="22" name="ACMPLP" queryTableFieldId="22" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{C74D06FB-AD56-4A98-983F-16DC10955D3B}" uniqueName="23" name="SLCDC" queryTableFieldId="23" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{24D5DD84-F585-4F0A-AD0F-1604A8FD60A9}" uniqueName="24" name="CTSU" queryTableFieldId="24" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2145,7 +2146,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2251,7 +2252,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2393,7 +2394,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>